<commit_message>
Started MVC on Homework 9
</commit_message>
<xml_diff>
--- a/Homework 9/Product Backlog.xlsx
+++ b/Homework 9/Product Backlog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/Project/Clas Diagram and Backlog/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/aaa2575_HW9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2748825C-D224-7645-A911-A393F30A52D7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7F1E6FA5-31FF-E547-8D17-596FC9EF2056}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="Sprint 5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="180">
   <si>
     <t>Product Name:</t>
   </si>
@@ -444,9 +443,6 @@
     <t>Wrap Up</t>
   </si>
   <si>
-    <t>Wrap_Up</t>
-  </si>
-  <si>
     <t>Delivery</t>
   </si>
   <si>
@@ -510,7 +506,70 @@
     <t>COM</t>
   </si>
   <si>
-    <t>Zip up code and uml and scrum spreadsheet</t>
+    <t>Add Methods to Library and Derived classes</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD </t>
+  </si>
+  <si>
+    <t>Add Methods to Transaction and Derived classes</t>
+  </si>
+  <si>
+    <t>Add Methods to Date and Derived classes</t>
+  </si>
+  <si>
+    <t>Write and compile empty Library class</t>
+  </si>
+  <si>
+    <t>Write and compile empty Transaction class</t>
+  </si>
+  <si>
+    <t>Write and compile empty Date class</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>Create menu propmts in view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Meun prompts in view </t>
+  </si>
+  <si>
+    <t>View</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Transaction</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Create Controller to implement MVC</t>
+  </si>
+  <si>
+    <t>Write and compile empty View</t>
+  </si>
+  <si>
+    <t>Write and compile empty Controller</t>
+  </si>
+  <si>
+    <t>Test MVC</t>
+  </si>
+  <si>
+    <t>Zip up code, uml and scrum spreadsheet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Save and Load functionality </t>
   </si>
 </sst>
 </file>
@@ -1600,28 +1659,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7070,8 +7129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7092,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -7103,7 +7162,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -7111,7 +7170,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -7310,7 +7369,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
@@ -7337,14 +7396,14 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B22" s="4">
         <f>B21+1</f>
         <v>2</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D22" s="4">
         <v>1</v>
@@ -7371,14 +7430,14 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B23" s="4">
         <f t="shared" ref="B23:B48" si="0">B22+1</f>
         <v>3</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D23" s="4">
         <v>1</v>
@@ -7405,14 +7464,14 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B24" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D24" s="4">
         <v>1</v>
@@ -8096,8 +8155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8240,13 +8299,13 @@
         <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F18" t="s">
         <v>123</v>
       </c>
       <c r="G18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -8264,13 +8323,13 @@
         <v>125</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F19" t="s">
         <v>126</v>
       </c>
       <c r="G19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -8288,13 +8347,13 @@
         <v>125</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F20" t="s">
         <v>127</v>
       </c>
       <c r="G20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -8312,13 +8371,13 @@
         <v>128</v>
       </c>
       <c r="E21" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F21" t="s">
         <v>129</v>
       </c>
       <c r="G21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -8336,13 +8395,13 @@
         <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F22" t="s">
         <v>131</v>
       </c>
       <c r="G22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -8360,13 +8419,13 @@
         <v>125</v>
       </c>
       <c r="E23" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F23" t="s">
         <v>132</v>
       </c>
       <c r="G23" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -8384,13 +8443,13 @@
         <v>122</v>
       </c>
       <c r="E24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F24" t="s">
         <v>134</v>
       </c>
       <c r="G24" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -8408,13 +8467,13 @@
         <v>130</v>
       </c>
       <c r="E25" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F25" t="s">
         <v>133</v>
       </c>
       <c r="G25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -8423,7 +8482,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C26" t="s">
         <v>121</v>
@@ -8432,13 +8491,13 @@
         <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" t="s">
         <v>135</v>
       </c>
       <c r="G26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -8447,22 +8506,22 @@
         <v>10</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
         <v>125</v>
       </c>
       <c r="E27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -8471,22 +8530,22 @@
         <v>11</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D28" t="s">
         <v>125</v>
       </c>
       <c r="E28" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F28" t="s">
         <v>127</v>
       </c>
       <c r="G28" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -8495,22 +8554,22 @@
         <v>12</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C29" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
         <v>128</v>
       </c>
       <c r="E29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F29" t="s">
         <v>129</v>
       </c>
       <c r="G29" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -8519,22 +8578,22 @@
         <v>13</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D30" t="s">
         <v>130</v>
       </c>
       <c r="E30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F30" t="s">
         <v>131</v>
       </c>
       <c r="G30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -8543,22 +8602,22 @@
         <v>14</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D31" t="s">
         <v>125</v>
       </c>
       <c r="E31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F31" t="s">
         <v>132</v>
       </c>
       <c r="G31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -8567,22 +8626,22 @@
         <v>15</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D32" t="s">
         <v>130</v>
       </c>
       <c r="E32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F32" t="s">
         <v>133</v>
       </c>
       <c r="G32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -8591,7 +8650,7 @@
         <v>16</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C33" t="s">
         <v>121</v>
@@ -8600,13 +8659,13 @@
         <v>122</v>
       </c>
       <c r="E33" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -8615,22 +8674,22 @@
         <v>17</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D34" t="s">
         <v>125</v>
       </c>
       <c r="E34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -8639,22 +8698,22 @@
         <v>18</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D35" t="s">
         <v>125</v>
       </c>
       <c r="E35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F35" t="s">
         <v>127</v>
       </c>
       <c r="G35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -8663,22 +8722,22 @@
         <v>19</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D36" t="s">
         <v>128</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F36" t="s">
         <v>129</v>
       </c>
       <c r="G36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -8687,22 +8746,22 @@
         <v>20</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D37" t="s">
         <v>130</v>
       </c>
       <c r="E37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F37" t="s">
         <v>131</v>
       </c>
       <c r="G37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -8711,22 +8770,22 @@
         <v>21</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D38" t="s">
         <v>125</v>
       </c>
       <c r="E38" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" t="s">
         <v>132</v>
       </c>
       <c r="G38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -8735,22 +8794,22 @@
         <v>22</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D39" t="s">
         <v>130</v>
       </c>
       <c r="E39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F39" t="s">
         <v>133</v>
       </c>
       <c r="G39" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -8759,7 +8818,7 @@
         <v>23</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
         <v>121</v>
@@ -8768,13 +8827,13 @@
         <v>122</v>
       </c>
       <c r="E40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -8783,22 +8842,22 @@
         <v>24</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D41" t="s">
         <v>125</v>
       </c>
       <c r="E41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -8807,22 +8866,22 @@
         <v>25</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D42" t="s">
         <v>125</v>
       </c>
       <c r="E42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
         <v>127</v>
       </c>
       <c r="G42" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -8831,22 +8890,22 @@
         <v>26</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D43" t="s">
         <v>128</v>
       </c>
       <c r="E43" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F43" t="s">
         <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -8855,22 +8914,22 @@
         <v>27</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C44" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D44" t="s">
         <v>130</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F44" t="s">
         <v>131</v>
       </c>
       <c r="G44" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -8879,22 +8938,22 @@
         <v>28</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D45" t="s">
         <v>125</v>
       </c>
       <c r="E45" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F45" t="s">
         <v>132</v>
       </c>
       <c r="G45" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -8903,22 +8962,22 @@
         <v>29</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D46" t="s">
         <v>130</v>
       </c>
       <c r="E46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F46" t="s">
         <v>133</v>
       </c>
       <c r="G46" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -8927,25 +8986,25 @@
         <v>30</v>
       </c>
       <c r="B47" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" t="s">
+        <v>137</v>
+      </c>
+      <c r="E47" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" t="s">
         <v>139</v>
       </c>
-      <c r="C47" t="s">
-        <v>137</v>
-      </c>
-      <c r="D47" t="s">
-        <v>138</v>
-      </c>
-      <c r="E47" t="s">
-        <v>142</v>
-      </c>
-      <c r="F47" t="s">
-        <v>140</v>
-      </c>
       <c r="G47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H47" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -8957,15 +9016,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView zoomScale="113" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="113" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -8997,8 +9059,8 @@
         <v>43</v>
       </c>
       <c r="B5">
-        <f>COUNT(A15:A1000)</f>
-        <v>0</v>
+        <f>COUNT(A15:A1002)</f>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -9007,7 +9069,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" ref="B6:B12" si="0">B5</f>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -9016,7 +9078,7 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -9025,7 +9087,7 @@
       </c>
       <c r="B8" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -9034,7 +9096,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -9043,7 +9105,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -9052,7 +9114,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -9061,7 +9123,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -9090,8 +9152,755 @@
         <v>22</v>
       </c>
     </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D18" t="s">
+        <v>122</v>
+      </c>
+      <c r="E18" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <f>A18+1</f>
+        <v>2</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F19" t="s">
+        <v>163</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <f t="shared" ref="A20:A48" si="1">A19+1</f>
+        <v>3</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E20" t="s">
+        <v>141</v>
+      </c>
+      <c r="F20" t="s">
+        <v>127</v>
+      </c>
+      <c r="G20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D21" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C22" t="s">
+        <v>170</v>
+      </c>
+      <c r="D22" t="s">
+        <v>130</v>
+      </c>
+      <c r="E22" t="s">
+        <v>141</v>
+      </c>
+      <c r="F22" t="s">
+        <v>131</v>
+      </c>
+      <c r="G22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C23" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" t="s">
+        <v>132</v>
+      </c>
+      <c r="G23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C24" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+      <c r="E24" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" t="s">
+        <v>141</v>
+      </c>
+      <c r="F25" t="s">
+        <v>161</v>
+      </c>
+      <c r="G25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C26" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" t="s">
+        <v>164</v>
+      </c>
+      <c r="G26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C27" t="s">
+        <v>171</v>
+      </c>
+      <c r="D27" t="s">
+        <v>125</v>
+      </c>
+      <c r="E27" t="s">
+        <v>141</v>
+      </c>
+      <c r="F27" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C28" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C29" t="s">
+        <v>171</v>
+      </c>
+      <c r="D29" t="s">
+        <v>130</v>
+      </c>
+      <c r="E29" t="s">
+        <v>141</v>
+      </c>
+      <c r="F29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" t="s">
+        <v>171</v>
+      </c>
+      <c r="D30" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D31" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" t="s">
+        <v>134</v>
+      </c>
+      <c r="G31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s">
+        <v>122</v>
+      </c>
+      <c r="E32" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" t="s">
+        <v>141</v>
+      </c>
+      <c r="F33" t="s">
+        <v>165</v>
+      </c>
+      <c r="G33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D34" t="s">
+        <v>125</v>
+      </c>
+      <c r="E34" t="s">
+        <v>141</v>
+      </c>
+      <c r="F34" t="s">
+        <v>127</v>
+      </c>
+      <c r="G34" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" t="s">
+        <v>172</v>
+      </c>
+      <c r="D35" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D36" t="s">
+        <v>130</v>
+      </c>
+      <c r="E36" t="s">
+        <v>141</v>
+      </c>
+      <c r="F36" t="s">
+        <v>131</v>
+      </c>
+      <c r="G36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" t="s">
+        <v>141</v>
+      </c>
+      <c r="F37" t="s">
+        <v>132</v>
+      </c>
+      <c r="G37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C38" t="s">
+        <v>136</v>
+      </c>
+      <c r="D38" t="s">
+        <v>122</v>
+      </c>
+      <c r="E38" t="s">
+        <v>141</v>
+      </c>
+      <c r="F38" t="s">
+        <v>134</v>
+      </c>
+      <c r="G38" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" t="s">
+        <v>169</v>
+      </c>
+      <c r="D39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E39" t="s">
+        <v>141</v>
+      </c>
+      <c r="F39" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C40" t="s">
+        <v>169</v>
+      </c>
+      <c r="D40" t="s">
+        <v>125</v>
+      </c>
+      <c r="E40" t="s">
+        <v>141</v>
+      </c>
+      <c r="F40" t="s">
+        <v>175</v>
+      </c>
+      <c r="G40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" t="s">
+        <v>169</v>
+      </c>
+      <c r="D41" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" t="s">
+        <v>168</v>
+      </c>
+      <c r="G41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" t="s">
+        <v>136</v>
+      </c>
+      <c r="D42" t="s">
+        <v>122</v>
+      </c>
+      <c r="E42" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" t="s">
+        <v>134</v>
+      </c>
+      <c r="G42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E43" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" t="s">
+        <v>174</v>
+      </c>
+      <c r="G43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17" customHeight="1">
+      <c r="A44">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44" t="s">
+        <v>125</v>
+      </c>
+      <c r="E44" t="s">
+        <v>141</v>
+      </c>
+      <c r="F44" t="s">
+        <v>176</v>
+      </c>
+      <c r="G44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45" t="s">
+        <v>125</v>
+      </c>
+      <c r="E45" t="s">
+        <v>141</v>
+      </c>
+      <c r="F45" t="s">
+        <v>177</v>
+      </c>
+      <c r="G45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" t="s">
+        <v>125</v>
+      </c>
+      <c r="E46" t="s">
+        <v>141</v>
+      </c>
+      <c r="F46" t="s">
+        <v>179</v>
+      </c>
+      <c r="G46" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="C47" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" t="s">
+        <v>141</v>
+      </c>
+      <c r="F47" t="s">
+        <v>134</v>
+      </c>
+      <c r="G47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C48" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" t="s">
+        <v>137</v>
+      </c>
+      <c r="E48" t="s">
+        <v>141</v>
+      </c>
+      <c r="F48" t="s">
+        <v>139</v>
+      </c>
+      <c r="G48" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
About to implement MVC
</commit_message>
<xml_diff>
--- a/Homework 9/Product Backlog.xlsx
+++ b/Homework 9/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atafoabure/Desktop/aaa2575_HW9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7F1E6FA5-31FF-E547-8D17-596FC9EF2056}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2B3C62DF-02F3-0343-891F-FCD186C7A003}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="182">
   <si>
     <t>Product Name:</t>
   </si>
@@ -570,6 +570,12 @@
   </si>
   <si>
     <t xml:space="preserve">Test Save and Load functionality </t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Need to fix check in and check out for transaction</t>
   </si>
 </sst>
 </file>
@@ -1662,25 +1668,25 @@
                   <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>31</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>31</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>31</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7129,8 +7135,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7144,6 +7150,7 @@
     <col min="7" max="7" width="38.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="45.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="130.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -7502,9 +7509,12 @@
         <v>5</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>28</v>
+        <v>180</v>
       </c>
       <c r="D25" s="4">
+        <v>2</v>
+      </c>
+      <c r="E25" s="4">
         <v>2</v>
       </c>
       <c r="F25" t="s">
@@ -7529,7 +7539,7 @@
         <v>6</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>28</v>
+        <v>180</v>
       </c>
       <c r="D26" s="4">
         <v>2</v>
@@ -7576,6 +7586,9 @@
       <c r="J27" t="s">
         <v>93</v>
       </c>
+      <c r="K27" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="28" spans="1:11">
       <c r="B28">
@@ -7637,7 +7650,7 @@
         <v>10</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>28</v>
+        <v>180</v>
       </c>
       <c r="D30" s="4">
         <v>2</v>
@@ -8155,7 +8168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
@@ -9018,8 +9031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="113" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A11" zoomScale="113" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -9068,8 +9081,8 @@
         <v>44</v>
       </c>
       <c r="B6" s="1">
-        <f t="shared" ref="B6:B12" si="0">B5</f>
-        <v>31</v>
+        <f>B5-6</f>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -9077,8 +9090,8 @@
         <v>45</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f>B6-5</f>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -9086,8 +9099,8 @@
         <v>46</v>
       </c>
       <c r="B8" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f t="shared" ref="B6:B12" si="0">B7</f>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -9096,7 +9109,7 @@
       </c>
       <c r="B9" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -9105,7 +9118,7 @@
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -9114,7 +9127,7 @@
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -9123,7 +9136,7 @@
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -9364,7 +9377,7 @@
         <v>164</v>
       </c>
       <c r="G26" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -9388,7 +9401,7 @@
         <v>127</v>
       </c>
       <c r="G27" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -9412,7 +9425,7 @@
         <v>129</v>
       </c>
       <c r="G28" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -9436,7 +9449,7 @@
         <v>131</v>
       </c>
       <c r="G29" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -9460,7 +9473,7 @@
         <v>132</v>
       </c>
       <c r="G30" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -9508,7 +9521,7 @@
         <v>162</v>
       </c>
       <c r="G32" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -9532,7 +9545,7 @@
         <v>165</v>
       </c>
       <c r="G33" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -9556,7 +9569,7 @@
         <v>127</v>
       </c>
       <c r="G34" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -9580,7 +9593,7 @@
         <v>129</v>
       </c>
       <c r="G35" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -9604,7 +9617,7 @@
         <v>131</v>
       </c>
       <c r="G36" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -9628,7 +9641,7 @@
         <v>132</v>
       </c>
       <c r="G37" t="s">
-        <v>28</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:8">

</xml_diff>